<commit_message>
add of dynamic web diagrams
</commit_message>
<xml_diff>
--- a/Auto-Eval-ASI1-r1.xlsx
+++ b/Auto-Eval-ASI1-r1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B18A0D56-096A-4766-A2D3-B2CA7674F265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B6D34F-63AE-4EA6-87C4-6A15015B4595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -513,91 +513,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -968,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1226,7 +1142,7 @@
         <v>53</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N7" t="s">
         <v>53</v>
@@ -1278,7 +1194,7 @@
         <v>53</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="N8" t="s">
         <v>53</v>
@@ -1330,7 +1246,7 @@
         <v>53</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="N9" t="s">
         <v>53</v>
@@ -1382,7 +1298,7 @@
         <v>53</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="N10" t="s">
         <v>53</v>
@@ -1434,7 +1350,7 @@
         <v>53</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="N11" t="s">
         <v>53</v>
@@ -3692,56 +3608,36 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7:O35 D37:O54">
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+  <conditionalFormatting sqref="D37:R54 D7:R35">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"AB"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"B"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S4:U4">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="notEqual">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P7:R35 P37:R54">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
-      <formula>"A"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
-      <formula>"AB"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"B"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"C"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
-      <formula>"D"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:R35 D37:R54" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D37:R54 D7:R35" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1 xml:space="preserve"> Note</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>